<commit_message>
IN-912 clientstatus should be uppercase
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D68F56-5FE3-564E-B3B6-8A72361E272C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A724248B-2611-2B48-88EF-7F0B4CF0E55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -442,9 +442,6 @@
   </si>
   <si>
     <t>clientstatus</t>
-  </si>
-  <si>
-    <t>Active</t>
   </si>
   <si>
     <t>Set to Death recorded if death record. Handled by death mapping</t>
@@ -1148,6 +1145,9 @@
   <si>
     <t>client_phonenumbers</t>
   </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
 </sst>
 </file>
 
@@ -1371,10 +1371,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1592,95 +1592,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D997D636-B97D-7B46-AB7B-633501338BD2}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>329</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="C1" s="35" t="s">
         <v>330</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="34" t="s">
         <v>331</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="E1" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="F1" s="34" t="s">
         <v>333</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="G1" s="34" t="s">
         <v>334</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>335</v>
       </c>
-      <c r="H1" s="37" t="s">
+    </row>
+    <row r="2" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="34" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="36" t="s">
+      <c r="B2" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="D2" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="34" t="s">
         <v>338</v>
       </c>
-      <c r="D2" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="36" t="s">
+      <c r="F2" s="34" t="s">
         <v>339</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="H2" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="H2" s="36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="36" t="s">
+      <c r="B3" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>306</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>339</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="34" t="s">
         <v>341</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B4" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="34" t="s">
         <v>338</v>
       </c>
-      <c r="D3" s="36" t="s">
-        <v>307</v>
-      </c>
-      <c r="E3" s="36" t="s">
+      <c r="F4" s="34" t="s">
         <v>339</v>
       </c>
-      <c r="F3" s="36" t="s">
-        <v>340</v>
-      </c>
-      <c r="H3" s="36" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="36" t="s">
-        <v>342</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>338</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>339</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>340</v>
-      </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="34" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1696,9 +1699,9 @@
   </sheetPr>
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3358,8 +3361,8 @@
       <c r="E50" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F50" s="34"/>
-      <c r="G50" s="35"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="37"/>
       <c r="H50" s="4" t="s">
         <v>30</v>
       </c>
@@ -3436,15 +3439,15 @@
       <c r="E52" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F52" s="34"/>
-      <c r="G52" s="35"/>
+      <c r="F52" s="36"/>
+      <c r="G52" s="37"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
       <c r="M52" s="4" t="s">
-        <v>109</v>
+        <v>342</v>
       </c>
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
@@ -3452,7 +3455,7 @@
         <v>22</v>
       </c>
       <c r="Q52" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3463,7 +3466,7 @@
         <v>18</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>29</v>
@@ -3480,7 +3483,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="6"/>
       <c r="N53" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O53" s="4"/>
       <c r="P53" s="4" t="s">
@@ -3496,7 +3499,7 @@
         <v>18</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>27</v>
@@ -3527,7 +3530,7 @@
         <v>18</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>27</v>
@@ -3558,7 +3561,7 @@
         <v>18</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>27</v>
@@ -3589,7 +3592,7 @@
         <v>18</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>54</v>
@@ -3622,7 +3625,7 @@
         <v>18</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>27</v>
@@ -3653,7 +3656,7 @@
         <v>18</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>27</v>
@@ -3684,7 +3687,7 @@
         <v>18</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>27</v>
@@ -3715,7 +3718,7 @@
         <v>18</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>27</v>
@@ -3729,10 +3732,10 @@
         <v>30</v>
       </c>
       <c r="I61" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="J61" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
@@ -3752,7 +3755,7 @@
         <v>18</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>54</v>
@@ -3785,7 +3788,7 @@
         <v>18</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>54</v>
@@ -3818,7 +3821,7 @@
         <v>18</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>54</v>
@@ -3851,7 +3854,7 @@
         <v>18</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>54</v>
@@ -3884,7 +3887,7 @@
         <v>18</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>54</v>
@@ -3917,7 +3920,7 @@
         <v>18</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>20</v>
@@ -3948,7 +3951,7 @@
         <v>18</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>27</v>
@@ -3979,7 +3982,7 @@
         <v>18</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>20</v>
@@ -4010,7 +4013,7 @@
         <v>18</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>54</v>
@@ -4043,7 +4046,7 @@
         <v>18</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>27</v>
@@ -4074,7 +4077,7 @@
         <v>18</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>27</v>
@@ -4105,7 +4108,7 @@
         <v>18</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>54</v>
@@ -4129,7 +4132,7 @@
         <v>47</v>
       </c>
       <c r="Q73" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4140,7 +4143,7 @@
         <v>18</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>27</v>
@@ -4148,8 +4151,8 @@
       <c r="E74" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F74" s="34"/>
-      <c r="G74" s="35"/>
+      <c r="F74" s="36"/>
+      <c r="G74" s="37"/>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
@@ -4171,7 +4174,7 @@
         <v>18</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>20</v>
@@ -4181,7 +4184,7 @@
       </c>
       <c r="F75" s="4"/>
       <c r="G75" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
@@ -4197,7 +4200,7 @@
         <v>47</v>
       </c>
       <c r="Q75" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4208,7 +4211,7 @@
         <v>18</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>27</v>
@@ -4216,15 +4219,15 @@
       <c r="E76" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F76" s="34"/>
-      <c r="G76" s="35"/>
+      <c r="F76" s="36"/>
+      <c r="G76" s="37"/>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
       <c r="M76" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N76" s="4"/>
       <c r="O76" s="4"/>
@@ -4241,7 +4244,7 @@
         <v>18</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>27</v>
@@ -4269,10 +4272,10 @@
         <v>17</v>
       </c>
       <c r="B78" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>20</v>
@@ -4283,15 +4286,15 @@
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
       <c r="H78" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I78" s="4"/>
       <c r="J78" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K78" s="4"/>
       <c r="L78" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M78" s="4"/>
       <c r="N78" s="4"/>
@@ -4309,7 +4312,7 @@
         <v>18</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>27</v>
@@ -4317,8 +4320,8 @@
       <c r="E79" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F79" s="34"/>
-      <c r="G79" s="35"/>
+      <c r="F79" s="36"/>
+      <c r="G79" s="37"/>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
@@ -4340,7 +4343,7 @@
         <v>18</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>59</v>
@@ -4357,7 +4360,7 @@
       <c r="L80" s="4"/>
       <c r="M80" s="4"/>
       <c r="N80" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O80" s="4"/>
       <c r="P80" s="4" t="s">
@@ -4373,7 +4376,7 @@
         <v>18</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>20</v>
@@ -5740,25 +5743,25 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="D1" s="16" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>154</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>34</v>
@@ -5785,16 +5788,16 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>152</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>153</v>
       </c>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
@@ -5823,7 +5826,7 @@
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2" s="11">
         <v>1</v>
@@ -12414,7 +12417,7 @@
     </row>
     <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>18</v>
@@ -12429,24 +12432,24 @@
         <v>1</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
       <c r="P2" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>20</v>
@@ -12455,7 +12458,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
@@ -12463,21 +12466,21 @@
         <v>99</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>27</v>
@@ -12489,20 +12492,20 @@
         <v>30</v>
       </c>
       <c r="I4" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>164</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>165</v>
       </c>
       <c r="N4" s="11"/>
       <c r="O4" s="11"/>
       <c r="P4" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>18</v>
@@ -12517,23 +12520,23 @@
         <v>0</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
       <c r="P5" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>54</v>
@@ -12547,18 +12550,18 @@
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
       <c r="P6" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>59</v>
@@ -12567,11 +12570,11 @@
         <v>0</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O7" s="11"/>
       <c r="P7" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -14022,16 +14025,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>152</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>153</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>16</v>
@@ -14041,264 +14044,264 @@
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>172</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>183</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>192</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>195</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="27" t="s">
         <v>198</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>199</v>
       </c>
       <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B17" s="25"/>
       <c r="C17" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>203</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B19" s="25"/>
       <c r="C19" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>208</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>213</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B22" s="25"/>
       <c r="C22" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B23" s="26"/>
       <c r="C23" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15771,127 +15774,127 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>153</v>
-      </c>
       <c r="E1" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B6" s="22"/>
       <c r="C6" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B7" s="22"/>
       <c r="C7" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B8" s="22"/>
       <c r="C8" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B10" s="22"/>
       <c r="C10" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -17328,16 +17331,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>152</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17346,10 +17349,10 @@
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>237</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17358,10 +17361,10 @@
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>239</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17370,10 +17373,10 @@
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17382,10 +17385,10 @@
       </c>
       <c r="B5" s="28"/>
       <c r="C5" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>243</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17394,10 +17397,10 @@
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>245</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17406,10 +17409,10 @@
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>247</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17418,10 +17421,10 @@
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>249</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17430,10 +17433,10 @@
       </c>
       <c r="B9" s="28"/>
       <c r="C9" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>251</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17442,10 +17445,10 @@
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>253</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17454,10 +17457,10 @@
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>255</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17466,10 +17469,10 @@
       </c>
       <c r="B12" s="28"/>
       <c r="C12" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>257</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17478,10 +17481,10 @@
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>259</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17490,10 +17493,10 @@
       </c>
       <c r="B14" s="28"/>
       <c r="C14" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>261</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17502,10 +17505,10 @@
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>263</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17514,10 +17517,10 @@
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>265</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17526,10 +17529,10 @@
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>267</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17538,10 +17541,10 @@
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>269</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17550,10 +17553,10 @@
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>271</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17562,10 +17565,10 @@
       </c>
       <c r="B20" s="28"/>
       <c r="C20" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>273</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17574,10 +17577,10 @@
       </c>
       <c r="B21" s="28"/>
       <c r="C21" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>275</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17586,10 +17589,10 @@
       </c>
       <c r="B22" s="28"/>
       <c r="C22" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>277</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17598,10 +17601,10 @@
       </c>
       <c r="B23" s="28"/>
       <c r="C23" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>279</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -17610,10 +17613,10 @@
       </c>
       <c r="B24" s="28"/>
       <c r="C24" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>281</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -17622,10 +17625,10 @@
       </c>
       <c r="B25" s="28"/>
       <c r="C25" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>283</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17634,10 +17637,10 @@
       </c>
       <c r="B26" s="28"/>
       <c r="C26" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>285</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17646,10 +17649,10 @@
       </c>
       <c r="B27" s="28"/>
       <c r="C27" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>287</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17658,10 +17661,10 @@
       </c>
       <c r="B28" s="28"/>
       <c r="C28" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>289</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17670,10 +17673,10 @@
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>291</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17682,10 +17685,10 @@
       </c>
       <c r="B30" s="28"/>
       <c r="C30" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="D30" s="11" t="s">
         <v>293</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17694,10 +17697,10 @@
       </c>
       <c r="B31" s="28"/>
       <c r="C31" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>295</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17706,10 +17709,10 @@
       </c>
       <c r="B32" s="28"/>
       <c r="C32" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>297</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17718,10 +17721,10 @@
       </c>
       <c r="B33" s="28"/>
       <c r="C33" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>299</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17730,10 +17733,10 @@
       </c>
       <c r="B34" s="28"/>
       <c r="C34" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>301</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17742,10 +17745,10 @@
       </c>
       <c r="B35" s="28"/>
       <c r="C35" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>303</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17754,10 +17757,10 @@
       </c>
       <c r="B36" s="28"/>
       <c r="C36" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>305</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -19273,7 +19276,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>18</v>
@@ -19288,7 +19291,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
@@ -19300,7 +19303,7 @@
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
       <c r="P2" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q2" s="30"/>
       <c r="R2" s="17"/>
@@ -19315,13 +19318,13 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>20</v>
@@ -19331,7 +19334,7 @@
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
@@ -19344,10 +19347,10 @@
         <v>99</v>
       </c>
       <c r="P3" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q3" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
@@ -19361,16 +19364,16 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="D4" s="30" t="s">
         <v>309</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>310</v>
       </c>
       <c r="E4" s="31" t="b">
         <v>0</v>
@@ -19381,20 +19384,20 @@
         <v>30</v>
       </c>
       <c r="I4" s="30" t="s">
+        <v>310</v>
+      </c>
+      <c r="J4" s="30" t="s">
         <v>311</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="K4" s="30" t="s">
         <v>312</v>
-      </c>
-      <c r="K4" s="30" t="s">
-        <v>313</v>
       </c>
       <c r="L4" s="30"/>
       <c r="M4" s="30"/>
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
       <c r="P4" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q4" s="30"/>
       <c r="R4" s="17"/>
@@ -19409,13 +19412,13 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D5" s="30" t="s">
         <v>27</v>
@@ -19429,10 +19432,10 @@
         <v>30</v>
       </c>
       <c r="I5" s="32" t="s">
+        <v>314</v>
+      </c>
+      <c r="J5" s="32" t="s">
         <v>315</v>
-      </c>
-      <c r="J5" s="32" t="s">
-        <v>316</v>
       </c>
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
@@ -19440,7 +19443,7 @@
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
       <c r="P5" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q5" s="30"/>
       <c r="R5" s="17"/>
@@ -19455,13 +19458,13 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D6" s="30" t="s">
         <v>27</v>
@@ -19475,10 +19478,10 @@
         <v>30</v>
       </c>
       <c r="I6" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="J6" s="32" t="s">
         <v>318</v>
-      </c>
-      <c r="J6" s="32" t="s">
-        <v>319</v>
       </c>
       <c r="K6" s="30"/>
       <c r="L6" s="30"/>
@@ -19486,7 +19489,7 @@
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
       <c r="P6" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q6" s="30"/>
       <c r="R6" s="17"/>
@@ -19501,13 +19504,13 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D7" s="30" t="s">
         <v>27</v>
@@ -19521,10 +19524,10 @@
         <v>30</v>
       </c>
       <c r="I7" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="J7" s="33" t="s">
         <v>321</v>
-      </c>
-      <c r="J7" s="33" t="s">
-        <v>322</v>
       </c>
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
@@ -19532,7 +19535,7 @@
       <c r="N7" s="30"/>
       <c r="O7" s="30"/>
       <c r="P7" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q7" s="30"/>
       <c r="R7" s="17"/>
@@ -19547,13 +19550,13 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>27</v>
@@ -19567,10 +19570,10 @@
         <v>30</v>
       </c>
       <c r="I8" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="J8" s="30" t="s">
         <v>121</v>
-      </c>
-      <c r="J8" s="30" t="s">
-        <v>122</v>
       </c>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
@@ -19578,7 +19581,7 @@
       <c r="N8" s="30"/>
       <c r="O8" s="30"/>
       <c r="P8" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q8" s="30"/>
       <c r="R8" s="17"/>
@@ -19593,7 +19596,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>18</v>
@@ -19615,12 +19618,12 @@
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
       <c r="M9" s="30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N9" s="30"/>
       <c r="O9" s="30"/>
       <c r="P9" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q9" s="30"/>
       <c r="R9" s="17"/>
@@ -19635,13 +19638,13 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>54</v>
@@ -19655,20 +19658,20 @@
         <v>30</v>
       </c>
       <c r="I10" s="30" t="s">
+        <v>325</v>
+      </c>
+      <c r="J10" s="30" t="s">
         <v>326</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="K10" s="30" t="s">
         <v>327</v>
-      </c>
-      <c r="K10" s="30" t="s">
-        <v>328</v>
       </c>
       <c r="L10" s="30"/>
       <c r="M10" s="30"/>
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
       <c r="P10" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q10" s="30"/>
       <c r="R10" s="17"/>

</xml_diff>

<commit_message>
IN-933 Add source condition for client and deputy phone numbers (#73)
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A724248B-2611-2B48-88EF-7F0B4CF0E55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7E5B12-6ED8-0B47-A7EE-9B86347C6BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="344">
   <si>
     <t>table_name</t>
   </si>
@@ -1148,6 +1148,9 @@
   <si>
     <t>ACTIVE</t>
   </si>
+  <si>
+    <t>Client Phone = not null</t>
+  </si>
 </sst>
 </file>
 
@@ -1592,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D997D636-B97D-7B46-AB7B-633501338BD2}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1682,6 +1685,9 @@
       </c>
       <c r="F4" s="34" t="s">
         <v>339</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>343</v>
       </c>
       <c r="H4" s="34" t="s">
         <v>99</v>
@@ -1699,7 +1705,7 @@
   </sheetPr>
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M52" sqref="M52"/>
     </sheetView>
@@ -12342,7 +12348,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add feepayer col (#74)
* add feepayer col

* overwrote status

* set a default of none on feepayer_id

* arg excel
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7E5B12-6ED8-0B47-A7EE-9B86347C6BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0AFCBF-C532-334D-8BD6-952FD4F3CA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="342">
   <si>
     <t>table_name</t>
   </si>
@@ -547,15 +547,6 @@
   </si>
   <si>
     <t>risk_score</t>
-  </si>
-  <si>
-    <t>CREC</t>
-  </si>
-  <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>crec_lookup</t>
   </si>
   <si>
     <t>caseactorgroup</t>
@@ -1149,6 +1140,9 @@
     <t>ACTIVE</t>
   </si>
   <si>
+    <t>none</t>
+  </si>
+  <si>
     <t>Client Phone = not null</t>
   </si>
 </sst>
@@ -1595,56 +1589,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D997D636-B97D-7B46-AB7B-633501338BD2}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>326</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1" s="34" t="s">
         <v>328</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="E1" s="34" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="F1" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="G1" s="34" t="s">
         <v>331</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="H1" s="35" t="s">
         <v>332</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>333</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>334</v>
-      </c>
-      <c r="H1" s="35" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="34" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D2" s="34" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H2" s="34" t="s">
         <v>37</v>
@@ -1652,19 +1643,19 @@
     </row>
     <row r="3" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="34" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H3" s="34" t="s">
         <v>99</v>
@@ -1672,22 +1663,22 @@
     </row>
     <row r="4" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>334</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>335</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="G4" s="34" t="s">
         <v>341</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>337</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>338</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>339</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>343</v>
       </c>
       <c r="H4" s="34" t="s">
         <v>99</v>
@@ -1705,9 +1696,9 @@
   </sheetPr>
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M52" sqref="M52"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H78" sqref="H78:L78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3453,7 +3444,7 @@
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
       <c r="M52" s="4" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
@@ -4003,11 +3994,13 @@
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
+      <c r="M69" s="4" t="s">
+        <v>340</v>
+      </c>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
       <c r="P69" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q69" s="4"/>
     </row>
@@ -4291,17 +4284,11 @@
       </c>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
-      <c r="H78" s="4" t="s">
-        <v>144</v>
-      </c>
+      <c r="H78" s="4"/>
       <c r="I78" s="4"/>
-      <c r="J78" s="4" t="s">
-        <v>145</v>
-      </c>
+      <c r="J78" s="4"/>
       <c r="K78" s="4"/>
-      <c r="L78" s="12" t="s">
-        <v>146</v>
-      </c>
+      <c r="L78" s="12"/>
       <c r="M78" s="4"/>
       <c r="N78" s="4"/>
       <c r="O78" s="4"/>
@@ -4318,7 +4305,7 @@
         <v>18</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>27</v>
@@ -4349,7 +4336,7 @@
         <v>18</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>59</v>
@@ -4382,7 +4369,7 @@
         <v>18</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>20</v>
@@ -5749,25 +5736,25 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>34</v>
@@ -5794,16 +5781,16 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
@@ -5832,7 +5819,7 @@
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D2" s="11">
         <v>1</v>
@@ -12348,7 +12335,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12423,7 +12410,7 @@
     </row>
     <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>18</v>
@@ -12438,24 +12425,24 @@
         <v>1</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
       <c r="P2" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>20</v>
@@ -12464,7 +12451,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
@@ -12472,21 +12459,21 @@
         <v>99</v>
       </c>
       <c r="P3" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q3" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>27</v>
@@ -12498,20 +12485,20 @@
         <v>30</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="N4" s="11"/>
       <c r="O4" s="11"/>
       <c r="P4" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>18</v>
@@ -12526,23 +12513,23 @@
         <v>0</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
       <c r="P5" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>54</v>
@@ -12556,18 +12543,18 @@
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
       <c r="P6" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>59</v>
@@ -12580,7 +12567,7 @@
       </c>
       <c r="O7" s="11"/>
       <c r="P7" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -14031,16 +14018,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>16</v>
@@ -14050,264 +14037,264 @@
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="25" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="22" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="25" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="22" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="26" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="22" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="22" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="22" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="25" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="22" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="25" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="22" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="22" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="22" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="25" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="22" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B17" s="25"/>
       <c r="C17" s="22" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="22" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B19" s="25"/>
       <c r="C19" s="22" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="22" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="25" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B22" s="25"/>
       <c r="C22" s="22" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="26" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B23" s="26"/>
       <c r="C23" s="22" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15780,127 +15767,127 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="22" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="22" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="22" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="22" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="22" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B6" s="22"/>
       <c r="C6" s="22" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B7" s="22"/>
       <c r="C7" s="22" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="22" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B8" s="22"/>
       <c r="C8" s="22" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="22" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="22" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="22" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B10" s="22"/>
       <c r="C10" s="22" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -17337,16 +17324,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="21" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17355,10 +17342,10 @@
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="13" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17367,10 +17354,10 @@
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="13" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17379,10 +17366,10 @@
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="13" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17391,10 +17378,10 @@
       </c>
       <c r="B5" s="28"/>
       <c r="C5" s="13" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17403,10 +17390,10 @@
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="13" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17415,10 +17402,10 @@
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="13" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17427,10 +17414,10 @@
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="13" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17439,10 +17426,10 @@
       </c>
       <c r="B9" s="28"/>
       <c r="C9" s="13" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17451,10 +17438,10 @@
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="13" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17463,10 +17450,10 @@
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="13" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17475,10 +17462,10 @@
       </c>
       <c r="B12" s="28"/>
       <c r="C12" s="13" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17487,10 +17474,10 @@
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="13" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17499,10 +17486,10 @@
       </c>
       <c r="B14" s="28"/>
       <c r="C14" s="13" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17511,10 +17498,10 @@
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="13" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17523,10 +17510,10 @@
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="13" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17535,10 +17522,10 @@
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="13" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17547,10 +17534,10 @@
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="13" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17559,10 +17546,10 @@
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="13" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -17571,10 +17558,10 @@
       </c>
       <c r="B20" s="28"/>
       <c r="C20" s="13" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17583,10 +17570,10 @@
       </c>
       <c r="B21" s="28"/>
       <c r="C21" s="13" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17595,10 +17582,10 @@
       </c>
       <c r="B22" s="28"/>
       <c r="C22" s="13" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17607,10 +17594,10 @@
       </c>
       <c r="B23" s="28"/>
       <c r="C23" s="13" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -17619,10 +17606,10 @@
       </c>
       <c r="B24" s="28"/>
       <c r="C24" s="13" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -17631,10 +17618,10 @@
       </c>
       <c r="B25" s="28"/>
       <c r="C25" s="13" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17643,10 +17630,10 @@
       </c>
       <c r="B26" s="28"/>
       <c r="C26" s="13" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17655,10 +17642,10 @@
       </c>
       <c r="B27" s="28"/>
       <c r="C27" s="13" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17667,10 +17654,10 @@
       </c>
       <c r="B28" s="28"/>
       <c r="C28" s="13" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17679,10 +17666,10 @@
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="13" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17691,10 +17678,10 @@
       </c>
       <c r="B30" s="28"/>
       <c r="C30" s="13" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17703,10 +17690,10 @@
       </c>
       <c r="B31" s="28"/>
       <c r="C31" s="13" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17715,10 +17702,10 @@
       </c>
       <c r="B32" s="28"/>
       <c r="C32" s="13" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17727,10 +17714,10 @@
       </c>
       <c r="B33" s="28"/>
       <c r="C33" s="13" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17739,10 +17726,10 @@
       </c>
       <c r="B34" s="28"/>
       <c r="C34" s="13" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17751,10 +17738,10 @@
       </c>
       <c r="B35" s="28"/>
       <c r="C35" s="13" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17763,10 +17750,10 @@
       </c>
       <c r="B36" s="28"/>
       <c r="C36" s="13" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -19282,7 +19269,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>18</v>
@@ -19297,7 +19284,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
@@ -19309,7 +19296,7 @@
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
       <c r="P2" s="30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q2" s="30"/>
       <c r="R2" s="17"/>
@@ -19324,13 +19311,13 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>20</v>
@@ -19340,7 +19327,7 @@
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
@@ -19353,10 +19340,10 @@
         <v>99</v>
       </c>
       <c r="P3" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q3" s="30" t="s">
         <v>158</v>
-      </c>
-      <c r="Q3" s="30" t="s">
-        <v>161</v>
       </c>
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
@@ -19370,16 +19357,16 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E4" s="31" t="b">
         <v>0</v>
@@ -19390,20 +19377,20 @@
         <v>30</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="J4" s="30" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="K4" s="30" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="L4" s="30"/>
       <c r="M4" s="30"/>
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
       <c r="P4" s="30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q4" s="30"/>
       <c r="R4" s="17"/>
@@ -19418,13 +19405,13 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D5" s="30" t="s">
         <v>27</v>
@@ -19438,10 +19425,10 @@
         <v>30</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
@@ -19449,7 +19436,7 @@
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
       <c r="P5" s="30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q5" s="30"/>
       <c r="R5" s="17"/>
@@ -19464,13 +19451,13 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D6" s="30" t="s">
         <v>27</v>
@@ -19484,10 +19471,10 @@
         <v>30</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="J6" s="32" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="K6" s="30"/>
       <c r="L6" s="30"/>
@@ -19495,7 +19482,7 @@
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
       <c r="P6" s="30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q6" s="30"/>
       <c r="R6" s="17"/>
@@ -19510,13 +19497,13 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D7" s="30" t="s">
         <v>27</v>
@@ -19530,10 +19517,10 @@
         <v>30</v>
       </c>
       <c r="I7" s="33" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="J7" s="33" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
@@ -19541,7 +19528,7 @@
       <c r="N7" s="30"/>
       <c r="O7" s="30"/>
       <c r="P7" s="30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q7" s="30"/>
       <c r="R7" s="17"/>
@@ -19556,13 +19543,13 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>27</v>
@@ -19587,7 +19574,7 @@
       <c r="N8" s="30"/>
       <c r="O8" s="30"/>
       <c r="P8" s="30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q8" s="30"/>
       <c r="R8" s="17"/>
@@ -19602,7 +19589,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>18</v>
@@ -19624,12 +19611,12 @@
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
       <c r="M9" s="30" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="N9" s="30"/>
       <c r="O9" s="30"/>
       <c r="P9" s="30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q9" s="30"/>
       <c r="R9" s="17"/>
@@ -19644,13 +19631,13 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>54</v>
@@ -19664,20 +19651,20 @@
         <v>30</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="J10" s="30" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="K10" s="30" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="L10" s="30"/>
       <c r="M10" s="30"/>
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
       <c r="P10" s="30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q10" s="30"/>
       <c r="R10" s="17"/>

</xml_diff>

<commit_message>
Set CASE-PILOT-ONE default value on client.caseactorgroup
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Client.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0AFCBF-C532-334D-8BD6-952FD4F3CA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B6CF0D-FC87-4440-A71B-37D4CA806132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -40,6 +40,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>added col name
 	-Jennifer Mackown</t>
@@ -53,6 +54,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>removed "no", not required
 	-Jennifer Mackown</t>
@@ -66,6 +68,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>removed "unknown"
 	-Jennifer Mackown</t>
@@ -79,6 +82,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>removed 'unique_number' - makes more sense as a calculation than a transformation
 	-Jennifer Mackown</t>
@@ -90,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="343">
   <si>
     <t>table_name</t>
   </si>
@@ -1145,6 +1149,9 @@
   <si>
     <t>Client Phone = not null</t>
   </si>
+  <si>
+    <t>CASE-PILOT-ONE</t>
+  </si>
 </sst>
 </file>
 
@@ -1164,52 +1171,62 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1698,7 +1715,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H78" sqref="H78:L78"/>
+      <selection pane="bottomLeft" activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4320,11 +4337,13 @@
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
-      <c r="M79" s="4"/>
+      <c r="M79" s="4" t="s">
+        <v>342</v>
+      </c>
       <c r="N79" s="4"/>
       <c r="O79" s="4"/>
       <c r="P79" s="4" t="s">
-        <v>25</v>
+        <v>155</v>
       </c>
       <c r="Q79" s="4"/>
     </row>

</xml_diff>